<commit_message>
Update lower avionics bulkhead. Added resized eyebolt to avionics assembly
</commit_message>
<xml_diff>
--- a/QRET_MechBOM_2019_20.xlsx
+++ b/QRET_MechBOM_2019_20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Graeme Barnes\Documents\GitHub\Repository Clone\MechComponents_02102012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52734D0A-7771-4EB0-A49D-1BBCB24A6042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274A2959-DFBB-4EAE-B226-9BC5C31F231B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{4CB8208B-D72B-40C0-8A49-185F68F2ED3A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4CB8208B-D72B-40C0-8A49-185F68F2ED3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Avionics" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="76">
   <si>
     <t>Component</t>
   </si>
@@ -259,6 +259,24 @@
   </si>
   <si>
     <t>Will be installed through the thrust plate, into the motor casing. Rated for 1300 lbs (vertical capacity).</t>
+  </si>
+  <si>
+    <t>3/4"-16 x 3/4" length Steel Eyebolt with shoulder</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/3014T954</t>
+  </si>
+  <si>
+    <t>This eyebolt is for the bottom avionics bulkhead and is rated for 1300 lbs.</t>
+  </si>
+  <si>
+    <t>Medium-Strength Steel Hex Nut - Grade 5, Zinc-Plated, 3/8"-16 thread size</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/95462a031</t>
+  </si>
+  <si>
+    <t>We need one nut to fasten the lower avionics bulkhead eyebolt</t>
   </si>
 </sst>
 </file>
@@ -357,7 +375,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -398,6 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -714,15 +733,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A74E661-9377-44F6-A771-BB2163B533D9}">
-  <dimension ref="B4:P17"/>
+  <dimension ref="B4:P19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N18" sqref="N17:N18"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.109375" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" customWidth="1"/>
     <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37" customWidth="1"/>
@@ -1040,7 +1059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>49</v>
       </c>
@@ -1058,6 +1077,52 @@
       </c>
       <c r="I17">
         <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="16">
+        <v>3.38</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="16">
+        <v>8.7899999999999991</v>
+      </c>
+      <c r="I19">
+        <v>100</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1071,9 +1136,11 @@
     <hyperlink ref="F15" r:id="rId7" xr:uid="{F7A9F219-EA1D-4F20-8872-EF2480010277}"/>
     <hyperlink ref="F16" r:id="rId8" xr:uid="{CFB7BA88-D23E-48D2-974E-001EABFE3186}"/>
     <hyperlink ref="F17" r:id="rId9" xr:uid="{0AB0E8AC-3EF2-4EFE-8EAF-5286D3510CC6}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{11E6C967-C354-4523-89D4-7DD93E383EFD}"/>
+    <hyperlink ref="F19" r:id="rId11" xr:uid="{969AC167-35A6-4BAE-9DFA-C9FB069852C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -1201,7 +1268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D421F24-F2B9-4156-970A-2DB29852D92A}">
   <dimension ref="C4:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update the upper avionics bulkhead and resized eyebolt.
</commit_message>
<xml_diff>
--- a/QRET_MechBOM_2019_20.xlsx
+++ b/QRET_MechBOM_2019_20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Graeme Barnes\Documents\GitHub\Repository Clone\MechComponents_02102012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274A2959-DFBB-4EAE-B226-9BC5C31F231B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D628A40-BE1A-43BF-B61B-0A088DFC960E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4CB8208B-D72B-40C0-8A49-185F68F2ED3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="82">
   <si>
     <t>Component</t>
   </si>
@@ -276,7 +276,49 @@
     <t>https://www.mcmaster.com/95462a031</t>
   </si>
   <si>
-    <t>We need one nut to fasten the lower avionics bulkhead eyebolt</t>
+    <t>5/16"-18 x 1-1/8" thread length, Steel Eyebolt with shoulder</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/3014t46</t>
+  </si>
+  <si>
+    <t>This eyebolt is for the upper avionics bulkhead. It is rated for 900 lbs.</t>
+  </si>
+  <si>
+    <t>Medium-Strength Steel Hex Nut - Grade 5, Zinc-Plated, 5/16"-18</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/95462a030</t>
+  </si>
+  <si>
+    <r>
+      <t>We need one nut to fasten the lower avionics bulkhead eyebolt **</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Check Home Depot - consider washer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Nut required for the upper avionics bulkhead. **</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Home Depot - consider washer</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -733,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A74E661-9377-44F6-A771-BB2163B533D9}">
-  <dimension ref="B4:P19"/>
+  <dimension ref="B4:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1122,7 +1164,53 @@
         <v>100</v>
       </c>
       <c r="N19" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="9" t="s">
         <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="16">
+        <v>3.45</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="16">
+        <v>7.18</v>
+      </c>
+      <c r="I21">
+        <v>100</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1138,9 +1226,11 @@
     <hyperlink ref="F17" r:id="rId9" xr:uid="{0AB0E8AC-3EF2-4EFE-8EAF-5286D3510CC6}"/>
     <hyperlink ref="F18" r:id="rId10" xr:uid="{11E6C967-C354-4523-89D4-7DD93E383EFD}"/>
     <hyperlink ref="F19" r:id="rId11" xr:uid="{969AC167-35A6-4BAE-9DFA-C9FB069852C4}"/>
+    <hyperlink ref="F20" r:id="rId12" xr:uid="{0DEB437A-3E7A-491A-94A7-E3E4ABF29E20}"/>
+    <hyperlink ref="F21" r:id="rId13" xr:uid="{2494426A-B9A9-4CFA-B0D9-96EE1150F490}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated avionincs bay BOM
</commit_message>
<xml_diff>
--- a/QRET_MechBOM_2019_20.xlsx
+++ b/QRET_MechBOM_2019_20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Graeme Barnes\Documents\GitHub\Repository Clone\MechComponents_02102012\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jshek\OneDrive\Documents\GitHub\MechComponents_02102012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D628A40-BE1A-43BF-B61B-0A088DFC960E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C70E14-5392-401F-AF4E-A858B853D949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4CB8208B-D72B-40C0-8A49-185F68F2ED3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4CB8208B-D72B-40C0-8A49-185F68F2ED3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Avionics" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="87">
   <si>
     <t>Component</t>
   </si>
@@ -151,9 +151,6 @@
     <t>https://www.mcmaster.com/95462a029</t>
   </si>
   <si>
-    <t>We may have these from last year</t>
-  </si>
-  <si>
     <t>316 Stainless Steel Washer - 
 for 1/4" Screw Size, 0.281" ID, 0.625" OD</t>
   </si>
@@ -192,13 +189,6 @@
   </si>
   <si>
     <t>9V Battery Holder Holder</t>
-  </si>
-  <si>
-    <t>3d Printed?</t>
-  </si>
-  <si>
-    <t>This is the red component that still
- needs to be figured out</t>
   </si>
   <si>
     <t>.</t>
@@ -319,6 +309,30 @@
       </rPr>
       <t>Home Depot - consider washer</t>
     </r>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>QRET Design Bay</t>
+  </si>
+  <si>
+    <t>Using last years</t>
+  </si>
+  <si>
+    <t>3d Printed</t>
+  </si>
+  <si>
+    <t>Red component Jamie is working on</t>
+  </si>
+  <si>
+    <t>Alloy Steel Low-Profile Socket Head Screw - Hex Drive, Black Oxide, 6-32 Thread Size, 1/2" Long</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92220a143</t>
+  </si>
+  <si>
+    <t>Radial screws for the bulk heads</t>
   </si>
 </sst>
 </file>
@@ -775,30 +789,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A74E661-9377-44F6-A771-BB2163B533D9}">
-  <dimension ref="B4:P21"/>
+  <dimension ref="B4:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.88671875" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="37.33203125" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.28515625" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
@@ -840,7 +854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
@@ -885,7 +899,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>24</v>
       </c>
@@ -908,7 +922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>29</v>
       </c>
@@ -928,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>34</v>
       </c>
@@ -946,7 +960,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>35</v>
       </c>
@@ -961,9 +975,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
         <v>31</v>
@@ -976,7 +990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="10" t="s">
         <v>36</v>
       </c>
@@ -990,7 +1004,7 @@
         <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="H11" s="13">
         <v>4.88</v>
@@ -999,12 +1013,15 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
+        <v>81</v>
+      </c>
+      <c r="P11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="C12" s="9" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C12" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="D12">
         <v>1.3</v>
@@ -1013,10 +1030,10 @@
         <v>15</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="H12" s="13">
         <v>7.11</v>
@@ -1025,18 +1042,21 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="P12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
         <v>42</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="G13" t="s">
         <v>28</v>
@@ -1048,28 +1068,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="F14" s="7"/>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
       <c r="H14" s="11"/>
+      <c r="I14">
+        <v>1</v>
+      </c>
       <c r="N14" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="G15" t="s">
         <v>28</v>
@@ -1081,15 +1107,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="G16" t="s">
         <v>28</v>
@@ -1101,15 +1127,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="G17" t="s">
         <v>28</v>
@@ -1121,15 +1147,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="3:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:14" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G18" t="s">
         <v>28</v>
@@ -1141,18 +1167,18 @@
         <v>1</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G19" t="s">
         <v>28</v>
@@ -1164,18 +1190,18 @@
         <v>100</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="3:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G20" t="s">
         <v>28</v>
@@ -1187,18 +1213,18 @@
         <v>1</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="3:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C21" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G21" t="s">
         <v>28</v>
@@ -1210,7 +1236,30 @@
         <v>100</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="C22" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="16">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1228,9 +1277,10 @@
     <hyperlink ref="F19" r:id="rId11" xr:uid="{969AC167-35A6-4BAE-9DFA-C9FB069852C4}"/>
     <hyperlink ref="F20" r:id="rId12" xr:uid="{0DEB437A-3E7A-491A-94A7-E3E4ABF29E20}"/>
     <hyperlink ref="F21" r:id="rId13" xr:uid="{2494426A-B9A9-4CFA-B0D9-96EE1150F490}"/>
+    <hyperlink ref="F22" r:id="rId14" xr:uid="{8B922BB3-9529-4525-BE2C-DF2461C425C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -1242,24 +1292,24 @@
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.33203125" customWidth="1"/>
-    <col min="17" max="17" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.28515625" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:17" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1362,20 +1412,20 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="30.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42.21875" customWidth="1"/>
-    <col min="17" max="17" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42.28515625" customWidth="1"/>
+    <col min="17" max="17" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1417,7 +1467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:17" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
@@ -1462,21 +1512,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="3:17" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I6" s="5">
         <v>10.54</v>
@@ -1485,32 +1535,32 @@
         <v>1</v>
       </c>
       <c r="K6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="3:17" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" ht="103.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I7" s="5">
         <v>3.89</v>
@@ -1519,32 +1569,32 @@
         <v>24</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="3:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D8" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I8" s="5">
         <v>4.09</v>
@@ -1553,46 +1603,46 @@
         <v>1</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="3:17" ht="57.6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" ht="60" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1615,20 +1665,20 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.28515625" customWidth="1"/>
     <col min="17" max="17" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1670,7 +1720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:17" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" ht="82.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>